<commit_message>
Added PDFs of slides.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox/School/Teaching/DATA606 2021 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE4B005-5930-9742-942B-BED16DF17FA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093BDDF2-F57E-9A4A-A165-4AD59566CFEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="8160" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>[Video](https://youtu.be/EUXDKpVLIY0), [Slides](/slides/08-Linear_Regression.html)</t>
+  </si>
+  <si>
+    <t>[Video](https://youtu.be/lo1ZEJIvOM4), [Slides](/slides/08-Linear_Regression2.html)</t>
   </si>
 </sst>
 </file>
@@ -602,7 +605,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,6 +860,9 @@
       </c>
       <c r="E13" t="s">
         <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>